<commit_message>
Padam template changes 12/08/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3B0B87-9CE2-4302-8C9F-7A6F25BEDBB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB32BF8D-7584-45AE-858C-A7C4ACB9B919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6003,13 +6003,13 @@
     <t>P[r]+N[r]</t>
   </si>
   <si>
-    <t>NRE/RE BP</t>
-  </si>
-  <si>
     <t>P[r]+S[r]</t>
   </si>
   <si>
     <t>P[r]+N[o]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRE/RE </t>
   </si>
 </sst>
 </file>
@@ -6717,10 +6717,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="D444" sqref="D444"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10354,7 +10354,7 @@
       <c r="S78" s="14"/>
       <c r="T78" s="14"/>
       <c r="U78" s="57" t="s">
-        <v>1991</v>
+        <v>1993</v>
       </c>
       <c r="V78" s="47"/>
     </row>
@@ -21968,7 +21968,7 @@
         <v>1888</v>
       </c>
       <c r="T377" s="7" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="U377" s="7"/>
       <c r="V377" s="47"/>
@@ -22319,7 +22319,7 @@
         <v>1888</v>
       </c>
       <c r="T386" s="7" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="U386" s="7"/>
       <c r="V386" s="47"/>

</xml_diff>

<commit_message>
TS 1.8 and 4.1 Padam input templates - 02/08/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D502A4EB-94F2-4F5E-8828-0E9AD7EBBCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 4.1'!$A$1:$XES$2294</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5832,7 +5833,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6583,13 +6584,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A869" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="W277" sqref="W277"/>
+      <selection pane="bottomLeft" activeCell="N854" sqref="N854"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -82997,7 +82998,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XES2294"/>
+  <autoFilter ref="A1:XES2294" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
nmv 14 08 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D502A4EB-94F2-4F5E-8828-0E9AD7EBBCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 4.1'!$A$1:$XES$2294</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5486,9 +5485,6 @@
     <t>iqhetIqha</t>
   </si>
   <si>
-    <t>aqgne itya#gne</t>
-  </si>
-  <si>
     <t>dAq iti# dAH</t>
   </si>
   <si>
@@ -5751,9 +5747,6 @@
   </si>
   <si>
     <t>Baqraqddhvaqmiti# Baraddhvam</t>
-  </si>
-  <si>
-    <t>maqKeByaqH iti# maqKeBya#H</t>
   </si>
   <si>
     <t>deqvAq iti# devAH</t>
@@ -5829,11 +5822,17 @@
       <t>qShya$m</t>
     </r>
   </si>
+  <si>
+    <t>aqgna itya#gne</t>
+  </si>
+  <si>
+    <t>maqKeByaq iti# maqKeBya#H</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6584,13 +6583,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A869" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2236" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N854" sqref="N854"/>
+      <selection pane="bottomLeft" activeCell="V2240" sqref="V2240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -8220,7 +8219,7 @@
         <v>91</v>
       </c>
       <c r="T28" s="14" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="U28" s="14"/>
       <c r="V28" s="45" t="s">
@@ -17922,7 +17921,7 @@
         <v>73</v>
       </c>
       <c r="N277" s="77" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="O277" s="6"/>
       <c r="P277" s="7"/>
@@ -22695,7 +22694,7 @@
     <row r="399" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A399" s="61"/>
       <c r="D399" s="74" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="E399" s="21"/>
       <c r="F399" s="21"/>
@@ -22740,7 +22739,7 @@
     <row r="400" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A400" s="61"/>
       <c r="D400" s="74" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="E400" s="21"/>
       <c r="F400" s="21"/>
@@ -29354,10 +29353,10 @@
       <c r="Q569" s="7"/>
       <c r="R569" s="7"/>
       <c r="S569" s="7" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="T569" s="7" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="U569" s="7"/>
       <c r="V569" s="45"/>
@@ -29743,10 +29742,10 @@
       <c r="Q579" s="7"/>
       <c r="R579" s="7"/>
       <c r="S579" s="7" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="T579" s="7" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="U579" s="7"/>
       <c r="V579" s="45"/>
@@ -34392,7 +34391,7 @@
       </c>
       <c r="R703" s="7"/>
       <c r="S703" s="7" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="T703" s="7" t="s">
         <v>155</v>
@@ -55072,8 +55071,8 @@
       <c r="U1318" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="V1318" s="45" t="s">
-        <v>1816</v>
+      <c r="V1318" s="46" t="s">
+        <v>1922</v>
       </c>
     </row>
     <row r="1319" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55422,7 +55421,7 @@
       <c r="Q1328" s="7"/>
       <c r="R1328" s="7"/>
       <c r="V1328" s="45" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="1329" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56091,7 +56090,7 @@
       <c r="Q1347" s="7"/>
       <c r="R1347" s="7"/>
       <c r="V1347" s="45" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="1348" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56408,7 +56407,7 @@
       <c r="Q1356" s="7"/>
       <c r="R1356" s="7"/>
       <c r="V1356" s="45" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="1357" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56710,7 +56709,7 @@
       <c r="Q1365" s="7"/>
       <c r="R1365" s="7"/>
       <c r="V1365" s="45" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="1366" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56959,7 +56958,7 @@
         <v>84</v>
       </c>
       <c r="V1372" s="45" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="1373" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57270,7 +57269,7 @@
       <c r="Q1381" s="7"/>
       <c r="R1381" s="7"/>
       <c r="V1381" s="45" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="1382" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57511,7 +57510,7 @@
       <c r="Q1388" s="7"/>
       <c r="R1388" s="7"/>
       <c r="V1388" s="45" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="1389" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57719,7 +57718,7 @@
       <c r="Q1394" s="7"/>
       <c r="R1394" s="7"/>
       <c r="V1394" s="45" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="1395" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57992,7 +57991,7 @@
       <c r="Q1402" s="7"/>
       <c r="R1402" s="7"/>
       <c r="V1402" s="45" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="1403" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58103,7 +58102,7 @@
       <c r="Q1405" s="7"/>
       <c r="R1405" s="7"/>
       <c r="V1405" s="45" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="1406" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58316,7 +58315,7 @@
       <c r="Q1411" s="7"/>
       <c r="R1411" s="7"/>
       <c r="V1411" s="45" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="1412" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58487,7 +58486,7 @@
       <c r="Q1416" s="7"/>
       <c r="R1416" s="7"/>
       <c r="V1416" s="45" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="1417" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58834,7 +58833,7 @@
       <c r="Q1426" s="7"/>
       <c r="R1426" s="7"/>
       <c r="V1426" s="45" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="1427" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59114,7 +59113,7 @@
       <c r="Q1434" s="7"/>
       <c r="R1434" s="7"/>
       <c r="V1434" s="45" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="1435" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59258,7 +59257,7 @@
       <c r="Q1438" s="7"/>
       <c r="R1438" s="7"/>
       <c r="V1438" s="45" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="1439" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59493,7 +59492,7 @@
       <c r="Q1445" s="7"/>
       <c r="R1445" s="7"/>
       <c r="S1445" s="7" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="T1445" s="7" t="s">
         <v>194</v>
@@ -59567,7 +59566,7 @@
       <c r="Q1447" s="7"/>
       <c r="R1447" s="7"/>
       <c r="V1447" s="45" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="1448" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59707,7 +59706,7 @@
       <c r="Q1451" s="7"/>
       <c r="R1451" s="7"/>
       <c r="V1451" s="45" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="1452" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59983,7 +59982,7 @@
         <v>174</v>
       </c>
       <c r="V1459" s="45" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="1460" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60092,7 +60091,7 @@
       <c r="Q1462" s="7"/>
       <c r="R1462" s="7"/>
       <c r="V1462" s="45" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="1463" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60342,7 +60341,7 @@
       <c r="Q1469" s="7"/>
       <c r="R1469" s="7"/>
       <c r="V1469" s="45" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="1470" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60830,7 +60829,7 @@
       <c r="Q1483" s="7"/>
       <c r="R1483" s="7"/>
       <c r="V1483" s="45" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="1484" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60935,7 +60934,7 @@
       <c r="Q1486" s="7"/>
       <c r="R1486" s="7"/>
       <c r="V1486" s="45" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="1487" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61249,7 +61248,7 @@
       <c r="Q1495" s="7"/>
       <c r="R1495" s="7"/>
       <c r="V1495" s="45" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="1496" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61319,7 +61318,7 @@
       <c r="Q1497" s="7"/>
       <c r="R1497" s="7"/>
       <c r="V1497" s="45" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="1498" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61556,7 +61555,7 @@
       <c r="Q1504" s="7"/>
       <c r="R1504" s="7"/>
       <c r="V1504" s="45" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="1505" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61774,7 +61773,7 @@
       <c r="Q1510" s="7"/>
       <c r="R1510" s="7"/>
       <c r="V1510" s="45" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="1511" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61981,7 +61980,7 @@
       <c r="Q1516" s="7"/>
       <c r="R1516" s="7"/>
       <c r="V1516" s="45" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="1517" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62118,7 +62117,7 @@
       <c r="Q1520" s="7"/>
       <c r="R1520" s="7"/>
       <c r="V1520" s="45" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="1521" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62338,7 +62337,7 @@
       <c r="Q1526" s="7"/>
       <c r="R1526" s="7"/>
       <c r="V1526" s="45" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="1527" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62507,7 +62506,7 @@
       <c r="Q1531" s="7"/>
       <c r="R1531" s="7"/>
       <c r="V1531" s="45" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="1532" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62836,7 +62835,7 @@
       <c r="Q1540" s="7"/>
       <c r="R1540" s="7"/>
       <c r="V1540" s="45" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="1541" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63159,7 +63158,7 @@
       <c r="Q1550" s="7"/>
       <c r="R1550" s="7"/>
       <c r="V1550" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1551" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63475,7 +63474,7 @@
       <c r="Q1559" s="7"/>
       <c r="R1559" s="7"/>
       <c r="V1559" s="45" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="1560" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63778,7 +63777,7 @@
       <c r="Q1568" s="7"/>
       <c r="R1568" s="7"/>
       <c r="V1568" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1569" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64086,7 +64085,7 @@
       <c r="Q1577" s="7"/>
       <c r="R1577" s="7"/>
       <c r="V1577" s="45" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="1578" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64319,7 +64318,7 @@
         <v>18</v>
       </c>
       <c r="V1586" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1587" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64551,7 +64550,7 @@
         <v>18</v>
       </c>
       <c r="V1595" s="45" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="1596" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64783,7 +64782,7 @@
         <v>18</v>
       </c>
       <c r="V1604" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1605" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64984,7 +64983,7 @@
         <v>18</v>
       </c>
       <c r="V1611" s="45" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="1612" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65226,7 +65225,7 @@
         <v>18</v>
       </c>
       <c r="V1620" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1621" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65712,7 +65711,7 @@
         <v>18</v>
       </c>
       <c r="V1639" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1640" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65968,7 +65967,7 @@
         <v>18</v>
       </c>
       <c r="V1649" s="45" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="1650" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66222,7 +66221,7 @@
         <v>18</v>
       </c>
       <c r="V1659" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1660" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66449,7 +66448,7 @@
         <v>18</v>
       </c>
       <c r="V1668" s="45" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="1669" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66703,7 +66702,7 @@
         <v>18</v>
       </c>
       <c r="V1678" s="45" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1679" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68063,7 +68062,7 @@
         <v>18</v>
       </c>
       <c r="V1732" s="45" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="1733" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68290,7 +68289,7 @@
         <v>18</v>
       </c>
       <c r="V1741" s="45" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="1742" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68583,7 +68582,7 @@
         <v>174</v>
       </c>
       <c r="V1752" s="45" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="1753" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68884,7 +68883,7 @@
         <v>18</v>
       </c>
       <c r="V1764" s="45" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="1765" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69021,7 +69020,7 @@
         <v>18</v>
       </c>
       <c r="V1769" s="45" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="1770" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69107,7 +69106,7 @@
         <v>129</v>
       </c>
       <c r="V1772" s="45" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="1773" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69315,7 +69314,7 @@
         <v>18</v>
       </c>
       <c r="V1779" s="45" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="1780" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69428,10 +69427,10 @@
         <v>1055</v>
       </c>
       <c r="S1783" s="7" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="T1783" s="7" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="V1783" s="45"/>
     </row>
@@ -69464,7 +69463,7 @@
         <v>18</v>
       </c>
       <c r="V1784" s="45" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="1785" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69640,7 +69639,7 @@
         <v>18</v>
       </c>
       <c r="V1790" s="45" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="1791" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69798,7 +69797,7 @@
         <v>18</v>
       </c>
       <c r="V1796" s="45" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="1797" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70031,7 +70030,7 @@
         <v>18</v>
       </c>
       <c r="V1805" s="45" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="1806" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70345,7 +70344,7 @@
         <v>18</v>
       </c>
       <c r="V1817" s="45" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="1818" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70527,7 +70526,7 @@
         <v>18</v>
       </c>
       <c r="V1824" s="45" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="1825" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70706,7 +70705,7 @@
         <v>18</v>
       </c>
       <c r="V1831" s="45" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="1832" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71153,7 +71152,7 @@
         <v>84</v>
       </c>
       <c r="V1848" s="45" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="1849" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71399,7 +71398,7 @@
         <v>18</v>
       </c>
       <c r="V1857" s="45" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="1858" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71596,7 +71595,7 @@
         <v>18</v>
       </c>
       <c r="V1865" s="45" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="1866" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71775,7 +71774,7 @@
         <v>174</v>
       </c>
       <c r="V1871" s="45" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="1872" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71975,7 +71974,7 @@
         <v>18</v>
       </c>
       <c r="V1879" s="45" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="1880" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72205,7 +72204,7 @@
         <v>18</v>
       </c>
       <c r="V1887" s="45" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="1888" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72465,7 +72464,7 @@
         <v>18</v>
       </c>
       <c r="V1897" s="45" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="1898" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72861,7 +72860,7 @@
         <v>18</v>
       </c>
       <c r="V1912" s="45" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="1913" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73022,7 +73021,7 @@
         <v>18</v>
       </c>
       <c r="V1918" s="45" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="1919" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73330,7 +73329,7 @@
         <v>18</v>
       </c>
       <c r="V1929" s="45" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="1930" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73472,7 +73471,7 @@
         <v>18</v>
       </c>
       <c r="V1934" s="45" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="1935" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73666,7 +73665,7 @@
         <v>18</v>
       </c>
       <c r="V1941" s="45" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="1942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73815,7 +73814,7 @@
         <v>18</v>
       </c>
       <c r="V1947" s="45" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="1948" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74002,7 +74001,7 @@
         <v>18</v>
       </c>
       <c r="V1954" s="45" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="1955" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74212,7 +74211,7 @@
         <v>18</v>
       </c>
       <c r="V1962" s="45" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="1963" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74437,7 +74436,7 @@
         <v>18</v>
       </c>
       <c r="V1971" s="45" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="1972" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74598,7 +74597,7 @@
         <v>18</v>
       </c>
       <c r="V1977" s="45" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="1978" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74783,7 +74782,7 @@
         <v>18</v>
       </c>
       <c r="V1984" s="45" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="1985" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75042,7 +75041,7 @@
         <v>18</v>
       </c>
       <c r="V1993" s="45" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="1994" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75235,7 +75234,7 @@
         <v>18</v>
       </c>
       <c r="V2000" s="45" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="2001" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75483,7 +75482,7 @@
         <v>18</v>
       </c>
       <c r="V2009" s="45" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="2010" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75722,7 +75721,7 @@
         <v>18</v>
       </c>
       <c r="V2018" s="45" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="2019" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75982,7 +75981,7 @@
         <v>18</v>
       </c>
       <c r="V2028" s="45" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="2029" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76110,7 +76109,7 @@
     </row>
     <row r="2034" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2034" s="56" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="I2034" s="48" t="s">
         <v>64</v>
@@ -76245,7 +76244,7 @@
         <v>18</v>
       </c>
       <c r="V2038" s="45" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="2039" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77323,7 +77322,7 @@
         <v>18</v>
       </c>
       <c r="V2079" s="45" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="2080" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77511,7 +77510,7 @@
         <v>18</v>
       </c>
       <c r="V2086" s="45" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="2087" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77691,7 +77690,7 @@
         <v>18</v>
       </c>
       <c r="V2093" s="45" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="2094" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77792,7 +77791,7 @@
         <v>18</v>
       </c>
       <c r="V2097" s="45" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="2098" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78072,7 +78071,7 @@
         <v>18</v>
       </c>
       <c r="V2108" s="45" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="2109" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78152,7 +78151,7 @@
         <v>18</v>
       </c>
       <c r="V2111" s="45" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="2112" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78560,7 +78559,7 @@
         <v>18</v>
       </c>
       <c r="V2127" s="45" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="2128" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78808,7 +78807,7 @@
         <v>18</v>
       </c>
       <c r="V2136" s="45" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="2137" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79067,7 +79066,7 @@
         <v>18</v>
       </c>
       <c r="V2146" s="45" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="2147" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79171,7 +79170,7 @@
         <v>18</v>
       </c>
       <c r="V2150" s="45" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="2151" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79248,7 +79247,7 @@
         <v>18</v>
       </c>
       <c r="V2153" s="45" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="2154" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79433,7 +79432,7 @@
         <v>18</v>
       </c>
       <c r="V2160" s="45" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79642,7 +79641,7 @@
         <v>18</v>
       </c>
       <c r="V2168" s="45" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="2169" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79845,7 +79844,7 @@
         <v>84</v>
       </c>
       <c r="V2176" s="45" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="2177" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79946,7 +79945,7 @@
         <v>18</v>
       </c>
       <c r="V2180" s="45" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="2181" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80234,7 +80233,7 @@
         <v>18</v>
       </c>
       <c r="V2191" s="45" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="2192" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80524,7 +80523,7 @@
         <v>18</v>
       </c>
       <c r="V2202" s="45" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="2203" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80829,7 +80828,7 @@
         <v>18</v>
       </c>
       <c r="V2212" s="45" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="2213" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81173,7 +81172,7 @@
         <v>18</v>
       </c>
       <c r="V2224" s="45" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="2225" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81382,7 +81381,7 @@
         <v>18</v>
       </c>
       <c r="V2232" s="45" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="2233" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81580,8 +81579,8 @@
       <c r="P2240" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="V2240" s="45" t="s">
-        <v>1905</v>
+      <c r="V2240" s="46" t="s">
+        <v>1923</v>
       </c>
     </row>
     <row r="2241" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81694,7 +81693,7 @@
         <v>18</v>
       </c>
       <c r="V2244" s="45" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="2245" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81875,7 +81874,7 @@
         <v>18</v>
       </c>
       <c r="V2251" s="45" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="2252" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81952,7 +81951,7 @@
         <v>18</v>
       </c>
       <c r="V2254" s="45" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="2255" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82163,7 +82162,7 @@
         <v>18</v>
       </c>
       <c r="V2262" s="45" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="2263" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82393,7 +82392,7 @@
         <v>18</v>
       </c>
       <c r="V2271" s="45" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="2272" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82527,7 +82526,7 @@
         <v>174</v>
       </c>
       <c r="V2276" s="45" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="2277" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82786,7 +82785,7 @@
         <v>18</v>
       </c>
       <c r="V2286" s="46" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="2287" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82890,7 +82889,7 @@
         <v>18</v>
       </c>
       <c r="V2290" s="45" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="2291" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -82998,7 +82997,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XES2294" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:XES2294"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TS 4.1 Ghanam split plus Template - 06/11/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CCBFCA-6DC5-4DA6-AFFC-363299CD2098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541642EB-29A4-4813-983D-85069914EDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 4.1'!$A$1:$V$2294</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6115,7 +6115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6328,24 +6328,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6647,7 +6629,7 @@
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S307" sqref="S307"/>
+      <selection pane="bottomLeft" activeCell="Q233" sqref="Q233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -43842,165 +43824,150 @@
     </row>
     <row r="1042" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1042" s="31"/>
-      <c r="I1042" s="73" t="s">
+      <c r="I1042" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="J1042" s="74">
+      <c r="J1042" s="42">
         <v>22</v>
       </c>
-      <c r="K1042" s="75">
+      <c r="K1042" s="5">
         <f t="shared" si="48"/>
         <v>1041</v>
       </c>
-      <c r="L1042" s="75">
+      <c r="L1042" s="5">
         <v>1</v>
       </c>
-      <c r="M1042" s="75">
+      <c r="M1042" s="5">
         <v>1</v>
       </c>
-      <c r="N1042" s="76" t="s">
+      <c r="N1042" s="40" t="s">
         <v>733</v>
       </c>
-      <c r="O1042" s="77"/>
-      <c r="P1042" s="78"/>
-      <c r="Q1042" s="78"/>
-      <c r="R1042" s="78"/>
-      <c r="S1042" s="78"/>
-      <c r="T1042" s="78"/>
-      <c r="U1042" s="78"/>
-      <c r="V1042" s="76" t="s">
+      <c r="O1042" s="6"/>
+      <c r="P1042" s="7"/>
+      <c r="Q1042" s="7"/>
+      <c r="R1042" s="7"/>
+      <c r="V1042" s="40" t="s">
         <v>1908</v>
       </c>
     </row>
     <row r="1043" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1043" s="73" t="s">
+      <c r="I1043" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="J1043" s="74">
+      <c r="J1043" s="42">
         <v>22</v>
       </c>
-      <c r="K1043" s="75">
+      <c r="K1043" s="5">
         <f t="shared" si="48"/>
         <v>1042</v>
       </c>
-      <c r="L1043" s="75">
+      <c r="L1043" s="5">
         <f t="shared" si="49"/>
         <v>2</v>
       </c>
-      <c r="M1043" s="75">
+      <c r="M1043" s="5">
         <f t="shared" si="50"/>
         <v>2</v>
       </c>
-      <c r="N1043" s="76" t="s">
+      <c r="N1043" s="40" t="s">
         <v>290</v>
       </c>
-      <c r="O1043" s="77"/>
-      <c r="P1043" s="78"/>
-      <c r="Q1043" s="78"/>
-      <c r="R1043" s="78"/>
-      <c r="S1043" s="78"/>
-      <c r="T1043" s="78"/>
-      <c r="U1043" s="78"/>
-      <c r="V1043" s="76" t="s">
+      <c r="O1043" s="6"/>
+      <c r="P1043" s="7"/>
+      <c r="Q1043" s="7"/>
+      <c r="R1043" s="7"/>
+      <c r="V1043" s="40" t="s">
         <v>1908</v>
       </c>
     </row>
     <row r="1044" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1044" s="73" t="s">
+      <c r="I1044" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="J1044" s="74">
+      <c r="J1044" s="42">
         <v>22</v>
       </c>
-      <c r="K1044" s="75">
+      <c r="K1044" s="5">
         <f t="shared" si="48"/>
         <v>1043</v>
       </c>
-      <c r="L1044" s="75">
+      <c r="L1044" s="5">
         <f t="shared" si="49"/>
         <v>3</v>
       </c>
-      <c r="M1044" s="75">
+      <c r="M1044" s="5">
         <f t="shared" si="50"/>
         <v>3</v>
       </c>
-      <c r="N1044" s="76" t="s">
+      <c r="N1044" s="40" t="s">
         <v>760</v>
       </c>
-      <c r="O1044" s="77"/>
-      <c r="P1044" s="78"/>
-      <c r="Q1044" s="78"/>
-      <c r="R1044" s="78"/>
-      <c r="S1044" s="78"/>
-      <c r="T1044" s="78"/>
-      <c r="U1044" s="78"/>
-      <c r="V1044" s="76" t="s">
+      <c r="O1044" s="6"/>
+      <c r="P1044" s="7"/>
+      <c r="Q1044" s="7"/>
+      <c r="R1044" s="7"/>
+      <c r="V1044" s="40" t="s">
         <v>1908</v>
       </c>
     </row>
     <row r="1045" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1045" s="73" t="s">
+      <c r="I1045" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="J1045" s="74">
+      <c r="J1045" s="42">
         <v>22</v>
       </c>
-      <c r="K1045" s="75">
+      <c r="K1045" s="5">
         <f t="shared" si="48"/>
         <v>1044</v>
       </c>
-      <c r="L1045" s="75">
+      <c r="L1045" s="5">
         <f t="shared" si="49"/>
         <v>4</v>
       </c>
-      <c r="M1045" s="75">
+      <c r="M1045" s="5">
         <f t="shared" si="50"/>
         <v>4</v>
       </c>
-      <c r="N1045" s="76" t="s">
+      <c r="N1045" s="40" t="s">
         <v>289</v>
       </c>
-      <c r="O1045" s="77"/>
-      <c r="P1045" s="78"/>
-      <c r="Q1045" s="78"/>
-      <c r="R1045" s="78"/>
-      <c r="S1045" s="78"/>
-      <c r="T1045" s="78"/>
-      <c r="U1045" s="78"/>
-      <c r="V1045" s="76" t="s">
+      <c r="O1045" s="6"/>
+      <c r="P1045" s="7"/>
+      <c r="Q1045" s="7"/>
+      <c r="R1045" s="7"/>
+      <c r="V1045" s="40" t="s">
         <v>1908</v>
       </c>
     </row>
     <row r="1046" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1046" s="73" t="s">
+      <c r="I1046" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="J1046" s="74">
+      <c r="J1046" s="42">
         <v>22</v>
       </c>
-      <c r="K1046" s="75">
+      <c r="K1046" s="5">
         <f t="shared" si="48"/>
         <v>1045</v>
       </c>
-      <c r="L1046" s="75">
+      <c r="L1046" s="5">
         <f t="shared" si="49"/>
         <v>5</v>
       </c>
-      <c r="M1046" s="75">
+      <c r="M1046" s="5">
         <f t="shared" si="50"/>
         <v>5</v>
       </c>
-      <c r="N1046" s="76" t="s">
+      <c r="N1046" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="O1046" s="77"/>
-      <c r="P1046" s="78"/>
-      <c r="Q1046" s="78"/>
-      <c r="R1046" s="78"/>
-      <c r="S1046" s="78"/>
-      <c r="T1046" s="78"/>
-      <c r="U1046" s="78"/>
-      <c r="V1046" s="76" t="s">
+      <c r="O1046" s="6"/>
+      <c r="P1046" s="7"/>
+      <c r="Q1046" s="7"/>
+      <c r="R1046" s="7"/>
+      <c r="V1046" s="40" t="s">
         <v>1908</v>
       </c>
     </row>
@@ -49201,14 +49168,14 @@
         <f t="shared" si="56"/>
         <v>3</v>
       </c>
-      <c r="N1213" s="80" t="s">
+      <c r="N1213" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1213" s="6"/>
       <c r="P1213" s="7"/>
       <c r="Q1213" s="7"/>
       <c r="R1213" s="7"/>
-      <c r="U1213" s="79" t="s">
+      <c r="U1213" s="73" t="s">
         <v>177</v>
       </c>
       <c r="V1213" s="40" t="s">
@@ -49800,14 +49767,14 @@
         <f t="shared" si="59"/>
         <v>22</v>
       </c>
-      <c r="N1232" s="80" t="s">
+      <c r="N1232" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1232" s="6"/>
       <c r="P1232" s="7"/>
       <c r="Q1232" s="7"/>
       <c r="R1232" s="7"/>
-      <c r="U1232" s="79" t="s">
+      <c r="U1232" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1232" s="40" t="s">
@@ -50264,7 +50231,7 @@
         <f t="shared" si="59"/>
         <v>36</v>
       </c>
-      <c r="N1246" s="80" t="s">
+      <c r="N1246" s="74" t="s">
         <v>336</v>
       </c>
       <c r="O1246" s="6"/>
@@ -50297,14 +50264,14 @@
         <f t="shared" si="59"/>
         <v>37</v>
       </c>
-      <c r="N1247" s="80" t="s">
+      <c r="N1247" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1247" s="6"/>
       <c r="P1247" s="7"/>
       <c r="Q1247" s="7"/>
       <c r="R1247" s="7"/>
-      <c r="U1247" s="79" t="s">
+      <c r="U1247" s="73" t="s">
         <v>178</v>
       </c>
       <c r="V1247" s="40" t="s">
@@ -50330,7 +50297,7 @@
         <f t="shared" si="59"/>
         <v>38</v>
       </c>
-      <c r="N1248" s="80" t="s">
+      <c r="N1248" s="74" t="s">
         <v>817</v>
       </c>
       <c r="O1248" s="6"/>
@@ -50480,7 +50447,7 @@
         <f t="shared" si="59"/>
         <v>43</v>
       </c>
-      <c r="N1253" s="80" t="s">
+      <c r="N1253" s="74" t="s">
         <v>252</v>
       </c>
       <c r="O1253" s="6"/>
@@ -50489,7 +50456,7 @@
       </c>
       <c r="Q1253" s="7"/>
       <c r="R1253" s="7"/>
-      <c r="U1253" s="79" t="s">
+      <c r="U1253" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1253" s="40" t="s">
@@ -50545,14 +50512,14 @@
         <f t="shared" si="59"/>
         <v>45</v>
       </c>
-      <c r="N1255" s="80" t="s">
+      <c r="N1255" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1255" s="6"/>
       <c r="P1255" s="7"/>
       <c r="Q1255" s="7"/>
       <c r="R1255" s="7"/>
-      <c r="U1255" s="79" t="s">
+      <c r="U1255" s="73" t="s">
         <v>177</v>
       </c>
       <c r="V1255" s="40" t="s">
@@ -50578,7 +50545,7 @@
         <f t="shared" si="59"/>
         <v>46</v>
       </c>
-      <c r="N1256" s="80" t="s">
+      <c r="N1256" s="74" t="s">
         <v>820</v>
       </c>
       <c r="O1256" s="6"/>
@@ -50668,7 +50635,7 @@
         <f t="shared" si="59"/>
         <v>49</v>
       </c>
-      <c r="N1259" s="80" t="s">
+      <c r="N1259" s="74" t="s">
         <v>624</v>
       </c>
       <c r="O1259" s="6"/>
@@ -50698,14 +50665,14 @@
         <f t="shared" si="59"/>
         <v>50</v>
       </c>
-      <c r="N1260" s="80" t="s">
+      <c r="N1260" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1260" s="6"/>
       <c r="P1260" s="7"/>
       <c r="Q1260" s="7"/>
       <c r="R1260" s="7"/>
-      <c r="U1260" s="79" t="s">
+      <c r="U1260" s="73" t="s">
         <v>178</v>
       </c>
       <c r="V1260" s="40" t="s">
@@ -51169,14 +51136,14 @@
         <f t="shared" si="59"/>
         <v>64</v>
       </c>
-      <c r="N1274" s="80" t="s">
+      <c r="N1274" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1274" s="6"/>
       <c r="P1274" s="7"/>
       <c r="Q1274" s="7"/>
       <c r="R1274" s="7"/>
-      <c r="U1274" s="79" t="s">
+      <c r="U1274" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1274" s="40" t="s">
@@ -51536,14 +51503,14 @@
         <f t="shared" si="62"/>
         <v>75</v>
       </c>
-      <c r="N1285" s="80" t="s">
+      <c r="N1285" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1285" s="6"/>
       <c r="P1285" s="7"/>
       <c r="Q1285" s="7"/>
       <c r="R1285" s="7"/>
-      <c r="U1285" s="79" t="s">
+      <c r="U1285" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1285" s="40" t="s">
@@ -51830,14 +51797,14 @@
         <f t="shared" si="62"/>
         <v>84</v>
       </c>
-      <c r="N1294" s="80" t="s">
+      <c r="N1294" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1294" s="6"/>
       <c r="P1294" s="7"/>
       <c r="Q1294" s="7"/>
       <c r="R1294" s="7"/>
-      <c r="U1294" s="79" t="s">
+      <c r="U1294" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1294" s="40" t="s">
@@ -51987,14 +51954,14 @@
         <f t="shared" si="62"/>
         <v>89</v>
       </c>
-      <c r="N1299" s="80" t="s">
+      <c r="N1299" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1299" s="6"/>
       <c r="P1299" s="7"/>
       <c r="Q1299" s="7"/>
       <c r="R1299" s="7"/>
-      <c r="U1299" s="79" t="s">
+      <c r="U1299" s="73" t="s">
         <v>177</v>
       </c>
       <c r="V1299" s="40" t="s">
@@ -52020,7 +51987,7 @@
         <f t="shared" si="62"/>
         <v>90</v>
       </c>
-      <c r="N1300" s="80" t="s">
+      <c r="N1300" s="74" t="s">
         <v>840</v>
       </c>
       <c r="O1300" s="7" t="s">
@@ -52208,14 +52175,14 @@
         <f t="shared" si="62"/>
         <v>96</v>
       </c>
-      <c r="N1306" s="80" t="s">
+      <c r="N1306" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1306" s="6"/>
       <c r="P1306" s="7"/>
       <c r="Q1306" s="7"/>
       <c r="R1306" s="7"/>
-      <c r="U1306" s="79" t="s">
+      <c r="U1306" s="73" t="s">
         <v>177</v>
       </c>
       <c r="V1306" s="40" t="s">
@@ -52241,7 +52208,7 @@
         <f t="shared" si="62"/>
         <v>97</v>
       </c>
-      <c r="N1307" s="80" t="s">
+      <c r="N1307" s="74" t="s">
         <v>845</v>
       </c>
       <c r="O1307" s="7" t="s">
@@ -52350,7 +52317,7 @@
       <c r="P1310" s="7"/>
       <c r="Q1310" s="7"/>
       <c r="R1310" s="7"/>
-      <c r="U1310" s="79" t="s">
+      <c r="U1310" s="73" t="s">
         <v>95</v>
       </c>
       <c r="V1310" s="40" t="s">
@@ -52621,7 +52588,7 @@
         <f t="shared" si="62"/>
         <v>108</v>
       </c>
-      <c r="N1318" s="80" t="s">
+      <c r="N1318" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1318" s="6"/>
@@ -52630,7 +52597,7 @@
       </c>
       <c r="Q1318" s="7"/>
       <c r="R1318" s="7"/>
-      <c r="U1318" s="79" t="s">
+      <c r="U1318" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1318" s="41" t="s">
@@ -52719,14 +52686,14 @@
         <f t="shared" si="62"/>
         <v>111</v>
       </c>
-      <c r="N1321" s="80" t="s">
+      <c r="N1321" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1321" s="6"/>
       <c r="P1321" s="7"/>
       <c r="Q1321" s="7"/>
       <c r="R1321" s="7"/>
-      <c r="U1321" s="79" t="s">
+      <c r="U1321" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1321" s="40" t="s">
@@ -53125,14 +53092,14 @@
         <f t="shared" si="62"/>
         <v>123</v>
       </c>
-      <c r="N1333" s="80" t="s">
+      <c r="N1333" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1333" s="6"/>
       <c r="P1333" s="7"/>
       <c r="Q1333" s="7"/>
       <c r="R1333" s="7"/>
-      <c r="U1333" s="79" t="s">
+      <c r="U1333" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1333" s="40" t="s">
@@ -54383,7 +54350,7 @@
         <f t="shared" si="65"/>
         <v>162</v>
       </c>
-      <c r="N1372" s="80" t="s">
+      <c r="N1372" s="74" t="s">
         <v>1603</v>
       </c>
       <c r="O1372" s="6"/>
@@ -54392,7 +54359,7 @@
       </c>
       <c r="Q1372" s="7"/>
       <c r="R1372" s="7"/>
-      <c r="U1372" s="79" t="s">
+      <c r="U1372" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1372" s="40" t="s">
@@ -54485,14 +54452,14 @@
         <f t="shared" si="65"/>
         <v>165</v>
       </c>
-      <c r="N1375" s="80" t="s">
+      <c r="N1375" s="74" t="s">
         <v>879</v>
       </c>
       <c r="O1375" s="6"/>
       <c r="P1375" s="7"/>
       <c r="Q1375" s="7"/>
       <c r="R1375" s="7"/>
-      <c r="U1375" s="79" t="s">
+      <c r="U1375" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1375" s="40" t="s">
@@ -54612,14 +54579,14 @@
         <f t="shared" si="65"/>
         <v>169</v>
       </c>
-      <c r="N1379" s="80" t="s">
+      <c r="N1379" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1379" s="6"/>
       <c r="P1379" s="7"/>
       <c r="Q1379" s="7"/>
       <c r="R1379" s="7"/>
-      <c r="U1379" s="79" t="s">
+      <c r="U1379" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1379" s="40" t="s">
@@ -55163,14 +55130,14 @@
         <f t="shared" si="65"/>
         <v>2</v>
       </c>
-      <c r="N1396" s="80" t="s">
+      <c r="N1396" s="74" t="s">
         <v>890</v>
       </c>
       <c r="O1396" s="6"/>
       <c r="P1396" s="7"/>
       <c r="Q1396" s="7"/>
       <c r="R1396" s="7"/>
-      <c r="U1396" s="79" t="s">
+      <c r="U1396" s="73" t="s">
         <v>95</v>
       </c>
       <c r="V1396" s="40" t="s">
@@ -55197,7 +55164,7 @@
         <f t="shared" si="65"/>
         <v>3</v>
       </c>
-      <c r="N1397" s="80" t="s">
+      <c r="N1397" s="74" t="s">
         <v>891</v>
       </c>
       <c r="O1397" s="7" t="s">
@@ -55524,14 +55491,14 @@
         <f t="shared" si="65"/>
         <v>13</v>
       </c>
-      <c r="N1407" s="80" t="s">
+      <c r="N1407" s="74" t="s">
         <v>898</v>
       </c>
       <c r="O1407" s="6"/>
       <c r="P1407" s="7"/>
       <c r="Q1407" s="7"/>
       <c r="R1407" s="7"/>
-      <c r="U1407" s="79" t="s">
+      <c r="U1407" s="73" t="s">
         <v>83</v>
       </c>
       <c r="V1407" s="40" t="s">
@@ -56001,7 +55968,7 @@
         <f t="shared" si="68"/>
         <v>28</v>
       </c>
-      <c r="N1422" s="80" t="s">
+      <c r="N1422" s="74" t="s">
         <v>465</v>
       </c>
       <c r="O1422" s="6"/>
@@ -56010,7 +55977,7 @@
       </c>
       <c r="Q1422" s="7"/>
       <c r="R1422" s="7"/>
-      <c r="U1422" s="79" t="s">
+      <c r="U1422" s="73" t="s">
         <v>1918</v>
       </c>
       <c r="V1422" s="40" t="s">
@@ -56435,14 +56402,14 @@
         <f t="shared" si="68"/>
         <v>41</v>
       </c>
-      <c r="N1435" s="80" t="s">
+      <c r="N1435" s="74" t="s">
         <v>199</v>
       </c>
       <c r="O1435" s="6"/>
       <c r="P1435" s="7"/>
       <c r="Q1435" s="7"/>
       <c r="R1435" s="7"/>
-      <c r="U1435" s="79" t="s">
+      <c r="U1435" s="73" t="s">
         <v>95</v>
       </c>
       <c r="V1435" s="40" t="s">
@@ -56469,7 +56436,7 @@
         <f t="shared" si="68"/>
         <v>42</v>
       </c>
-      <c r="N1436" s="80" t="s">
+      <c r="N1436" s="74" t="s">
         <v>911</v>
       </c>
       <c r="O1436" s="6"/>
@@ -56693,14 +56660,14 @@
         <f t="shared" si="68"/>
         <v>49</v>
       </c>
-      <c r="N1443" s="80" t="s">
+      <c r="N1443" s="74" t="s">
         <v>623</v>
       </c>
       <c r="O1443" s="7"/>
       <c r="P1443" s="7"/>
       <c r="Q1443" s="7"/>
       <c r="R1443" s="7"/>
-      <c r="U1443" s="79" t="s">
+      <c r="U1443" s="73" t="s">
         <v>95</v>
       </c>
       <c r="V1443" s="40" t="s">
@@ -56727,7 +56694,7 @@
         <f t="shared" si="68"/>
         <v>50</v>
       </c>
-      <c r="N1444" s="80" t="s">
+      <c r="N1444" s="74" t="s">
         <v>259</v>
       </c>
       <c r="O1444" s="6"/>
@@ -57081,14 +57048,14 @@
         <f t="shared" si="68"/>
         <v>61</v>
       </c>
-      <c r="N1455" s="80" t="s">
+      <c r="N1455" s="74" t="s">
         <v>890</v>
       </c>
       <c r="O1455" s="6"/>
       <c r="P1455" s="7"/>
       <c r="Q1455" s="7"/>
       <c r="R1455" s="7"/>
-      <c r="U1455" s="79" t="s">
+      <c r="U1455" s="73" t="s">
         <v>95</v>
       </c>
       <c r="V1455" s="40" t="s">
@@ -57115,7 +57082,7 @@
         <f t="shared" si="68"/>
         <v>62</v>
       </c>
-      <c r="N1456" s="80" t="s">
+      <c r="N1456" s="74" t="s">
         <v>243</v>
       </c>
       <c r="O1456" s="6"/>
@@ -57386,14 +57353,14 @@
         <f t="shared" si="68"/>
         <v>70</v>
       </c>
-      <c r="N1464" s="80" t="s">
+      <c r="N1464" s="74" t="s">
         <v>890</v>
       </c>
       <c r="O1464" s="6"/>
       <c r="P1464" s="7"/>
       <c r="Q1464" s="7"/>
       <c r="R1464" s="7"/>
-      <c r="U1464" s="79" t="s">
+      <c r="U1464" s="73" t="s">
         <v>1919</v>
       </c>
       <c r="V1464" s="40" t="s">
@@ -57420,7 +57387,7 @@
         <f t="shared" si="68"/>
         <v>71</v>
       </c>
-      <c r="N1465" s="80" t="s">
+      <c r="N1465" s="74" t="s">
         <v>925</v>
       </c>
       <c r="O1465" s="6" t="s">
@@ -57674,14 +57641,14 @@
         <f t="shared" si="68"/>
         <v>79</v>
       </c>
-      <c r="N1473" s="76" t="s">
+      <c r="N1473" s="40" t="s">
         <v>929</v>
       </c>
       <c r="O1473" s="6"/>
       <c r="P1473" s="7"/>
       <c r="Q1473" s="7"/>
       <c r="R1473" s="7"/>
-      <c r="U1473" s="78" t="s">
+      <c r="U1473" s="7" t="s">
         <v>95</v>
       </c>
       <c r="V1473" s="40" t="s">
@@ -57708,7 +57675,7 @@
         <f t="shared" si="68"/>
         <v>80</v>
       </c>
-      <c r="N1474" s="76" t="s">
+      <c r="N1474" s="40" t="s">
         <v>272</v>
       </c>
       <c r="O1474" s="7"/>
@@ -57717,7 +57684,6 @@
       </c>
       <c r="Q1474" s="7"/>
       <c r="R1474" s="7"/>
-      <c r="U1474" s="78"/>
       <c r="V1474" s="40" t="s">
         <v>1772</v>
       </c>
@@ -57743,14 +57709,13 @@
         <f t="shared" si="68"/>
         <v>81</v>
       </c>
-      <c r="N1475" s="76" t="s">
+      <c r="N1475" s="40" t="s">
         <v>930</v>
       </c>
       <c r="O1475" s="6"/>
       <c r="P1475" s="7"/>
       <c r="Q1475" s="7"/>
       <c r="R1475" s="7"/>
-      <c r="U1475" s="78"/>
       <c r="V1475" s="40" t="s">
         <v>1908</v>
       </c>
@@ -57776,14 +57741,13 @@
         <f t="shared" ref="M1476:M1539" si="71">+M1475+1</f>
         <v>82</v>
       </c>
-      <c r="N1476" s="76" t="s">
+      <c r="N1476" s="40" t="s">
         <v>931</v>
       </c>
       <c r="O1476" s="6"/>
       <c r="P1476" s="7"/>
       <c r="Q1476" s="7"/>
       <c r="R1476" s="7"/>
-      <c r="U1476" s="78"/>
       <c r="V1476" s="40" t="s">
         <v>1908</v>
       </c>
@@ -57811,14 +57775,13 @@
         <f t="shared" si="71"/>
         <v>83</v>
       </c>
-      <c r="N1477" s="76" t="s">
+      <c r="N1477" s="40" t="s">
         <v>932</v>
       </c>
       <c r="O1477" s="6"/>
       <c r="P1477" s="7"/>
       <c r="Q1477" s="7"/>
       <c r="R1477" s="7"/>
-      <c r="U1477" s="78"/>
       <c r="V1477" s="40" t="s">
         <v>1908</v>
       </c>
@@ -57846,14 +57809,14 @@
         <f t="shared" si="71"/>
         <v>84</v>
       </c>
-      <c r="N1478" s="76" t="s">
+      <c r="N1478" s="40" t="s">
         <v>929</v>
       </c>
       <c r="O1478" s="6"/>
       <c r="P1478" s="7"/>
       <c r="Q1478" s="7"/>
       <c r="R1478" s="7"/>
-      <c r="U1478" s="78" t="s">
+      <c r="U1478" s="7" t="s">
         <v>95</v>
       </c>
       <c r="V1478" s="40" t="s">
@@ -57883,7 +57846,7 @@
         <f t="shared" si="71"/>
         <v>85</v>
       </c>
-      <c r="N1479" s="76" t="s">
+      <c r="N1479" s="40" t="s">
         <v>272</v>
       </c>
       <c r="O1479" s="6"/>
@@ -61950,7 +61913,7 @@
         <f t="shared" si="77"/>
         <v>215</v>
       </c>
-      <c r="N1609" s="81" t="s">
+      <c r="N1609" s="75" t="s">
         <v>989</v>
       </c>
       <c r="O1609" s="7" t="s">
@@ -61983,7 +61946,7 @@
         <f t="shared" si="77"/>
         <v>216</v>
       </c>
-      <c r="N1610" s="81" t="s">
+      <c r="N1610" s="75" t="s">
         <v>204</v>
       </c>
       <c r="V1610" s="40" t="s">
@@ -67037,7 +67000,7 @@
         <f t="shared" si="83"/>
         <v>115</v>
       </c>
-      <c r="N1793" s="76" t="s">
+      <c r="N1793" s="40" t="s">
         <v>535</v>
       </c>
       <c r="V1793" s="40" t="s">
@@ -69298,10 +69261,10 @@
         <f t="shared" si="89"/>
         <v>26</v>
       </c>
-      <c r="N1874" s="76" t="s">
+      <c r="N1874" s="40" t="s">
         <v>581</v>
       </c>
-      <c r="U1874" s="78" t="s">
+      <c r="U1874" s="7" t="s">
         <v>95</v>
       </c>
       <c r="V1874" s="40" t="s">
@@ -69327,7 +69290,7 @@
         <f t="shared" si="89"/>
         <v>27</v>
       </c>
-      <c r="N1875" s="76" t="s">
+      <c r="N1875" s="40" t="s">
         <v>336</v>
       </c>
       <c r="V1875" s="40" t="s">
@@ -69839,7 +69802,7 @@
         <f t="shared" si="89"/>
         <v>45</v>
       </c>
-      <c r="N1893" s="76" t="s">
+      <c r="N1893" s="40" t="s">
         <v>535</v>
       </c>
       <c r="V1893" s="40" t="s">
@@ -70060,7 +70023,7 @@
       <c r="N1901" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="U1901" s="82" t="s">
+      <c r="U1901" s="76" t="s">
         <v>95</v>
       </c>
       <c r="V1901" s="40" t="s">
@@ -71454,7 +71417,7 @@
         <v>0</v>
       </c>
       <c r="P1950" s="14"/>
-      <c r="U1950" s="82" t="s">
+      <c r="U1950" s="76" t="s">
         <v>83</v>
       </c>
       <c r="V1950" s="40" t="s">
@@ -71656,7 +71619,7 @@
       <c r="N1957" s="72" t="s">
         <v>1126</v>
       </c>
-      <c r="U1957" s="82" t="s">
+      <c r="U1957" s="76" t="s">
         <v>95</v>
       </c>
       <c r="V1957" s="40" t="s">
@@ -72360,7 +72323,7 @@
       <c r="N1983" s="72" t="s">
         <v>1049</v>
       </c>
-      <c r="U1983" s="82" t="s">
+      <c r="U1983" s="76" t="s">
         <v>95</v>
       </c>
       <c r="V1983" s="40" t="s">
@@ -73161,7 +73124,7 @@
       <c r="N2010" s="72" t="s">
         <v>369</v>
       </c>
-      <c r="U2010" s="82" t="s">
+      <c r="U2010" s="76" t="s">
         <v>95</v>
       </c>
       <c r="V2010" s="40" t="s">
@@ -73190,7 +73153,7 @@
       <c r="N2011" s="72" t="s">
         <v>1150</v>
       </c>
-      <c r="U2011" s="82" t="s">
+      <c r="U2011" s="76" t="s">
         <v>83</v>
       </c>
       <c r="V2011" s="40" t="s">
@@ -73794,7 +73757,7 @@
         <f t="shared" si="95"/>
         <v>185</v>
       </c>
-      <c r="N2033" s="83" t="s">
+      <c r="N2033" s="77" t="s">
         <v>1160</v>
       </c>
       <c r="V2033" s="40" t="s">
@@ -73823,7 +73786,7 @@
         <f t="shared" si="95"/>
         <v>186</v>
       </c>
-      <c r="N2034" s="83" t="s">
+      <c r="N2034" s="77" t="s">
         <v>251</v>
       </c>
       <c r="O2034" s="6" t="s">

</xml_diff>

<commit_message>
nmv 16 11 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EED0813-CE6A-4679-937A-9F827C56AE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EEE035-715B-4DB3-B134-800F4A811BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6630,9 +6630,9 @@
   <dimension ref="A1:V2294"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A787" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1306" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U799" sqref="U799"/>
+      <selection pane="bottomLeft" activeCell="U1314" sqref="U1314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -52608,7 +52608,7 @@
       <c r="Q1318" s="7"/>
       <c r="R1318" s="7"/>
       <c r="U1318" s="73" t="s">
-        <v>83</v>
+        <v>177</v>
       </c>
       <c r="V1318" s="41" t="s">
         <v>1900</v>

</xml_diff>

<commit_message>
nmv 27 11 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA8BF1E-182C-4565-9F62-97483DBD4363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4EDC70-6FCE-4D96-9143-F1FCE997D77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8356" uniqueCount="1922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8357" uniqueCount="1922">
   <si>
     <t>PS</t>
   </si>
@@ -6645,9 +6645,9 @@
   <dimension ref="A1:V2294"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1511" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1643" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1524" sqref="V1524"/>
+      <selection pane="bottomLeft" activeCell="N1655" sqref="N1655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -63193,6 +63193,9 @@
       <c r="N1654" s="40" t="s">
         <v>1005</v>
       </c>
+      <c r="U1654" s="64" t="s">
+        <v>95</v>
+      </c>
       <c r="V1654" s="40" t="s">
         <v>1902</v>
       </c>

</xml_diff>

<commit_message>
nmv 24 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.1 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2497362-7A78-4123-AE6E-522034032232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5122DA6-7797-454E-B068-F12734AEC011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8360" uniqueCount="1922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8361" uniqueCount="1923">
   <si>
     <t>PS</t>
   </si>
@@ -5853,6 +5853,9 @@
   </si>
   <si>
     <t>te</t>
+  </si>
+  <si>
+    <t>S[r]</t>
   </si>
 </sst>
 </file>
@@ -6647,10 +6650,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2198" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A604" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2204" sqref="N2204"/>
+      <selection pane="bottomLeft" activeCell="U615" sqref="U615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -24630,8 +24633,12 @@
       <c r="P464" s="7"/>
       <c r="Q464" s="7"/>
       <c r="R464" s="7"/>
-      <c r="S464" s="7"/>
-      <c r="T464" s="7"/>
+      <c r="S464" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="T464" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="U464" s="70" t="s">
         <v>83</v>
       </c>
@@ -29196,8 +29203,12 @@
       <c r="P589" s="7"/>
       <c r="Q589" s="7"/>
       <c r="R589" s="7"/>
-      <c r="S589" s="7"/>
-      <c r="T589" s="7"/>
+      <c r="S589" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="T589" s="58" t="s">
+        <v>1922</v>
+      </c>
       <c r="U589" s="7"/>
       <c r="V589" s="40" t="s">
         <v>1892</v>
@@ -30142,7 +30153,9 @@
       <c r="R615" s="7"/>
       <c r="S615" s="7"/>
       <c r="T615" s="7"/>
-      <c r="U615" s="7"/>
+      <c r="U615" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="V615" s="40" t="s">
         <v>1334</v>
       </c>

</xml_diff>